<commit_message>
test: change files to import
</commit_message>
<xml_diff>
--- a/spec/fixtures/acoes.xlsx
+++ b/spec/fixtures/acoes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="33">
   <si>
     <t xml:space="preserve">Entrada/Saída</t>
   </si>
@@ -79,6 +79,18 @@
     <t xml:space="preserve">BEEF3 - MINERVA S/A</t>
   </si>
   <si>
+    <t xml:space="preserve">15/12/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dividendo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juros Sobre Capital Próprio</t>
+  </si>
+  <si>
     <t xml:space="preserve">12/08/2022</t>
   </si>
   <si>
@@ -98,6 +110,15 @@
   </si>
   <si>
     <t xml:space="preserve">ITSA4 - ITAUSA S/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26/08/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITSA4 - ITAUSA S.A.                                       </t>
   </si>
 </sst>
 </file>
@@ -181,7 +202,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -202,6 +223,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -219,13 +244,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="47.65"/>
@@ -365,7 +390,7 @@
         <v>68.5</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>8</v>
       </c>
@@ -373,7 +398,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>16</v>
@@ -381,40 +406,40 @@
       <c r="E6" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="3" t="n">
-        <v>25</v>
-      </c>
-      <c r="G6" s="4" t="n">
-        <v>37.15</v>
-      </c>
-      <c r="H6" s="4" t="n">
-        <v>928.75</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>4.39</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="G7" s="4" t="n">
-        <v>38.25</v>
-      </c>
-      <c r="H7" s="4" t="n">
-        <v>191.25</v>
+      <c r="G7" s="5" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>1.8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -434,39 +459,143 @@
         <v>12</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>150</v>
+        <v>25</v>
       </c>
       <c r="G8" s="4" t="n">
-        <v>32.89</v>
+        <v>37.15</v>
       </c>
       <c r="H8" s="4" t="n">
-        <v>4933.5</v>
+        <v>928.75</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="G9" s="4" t="n">
+        <v>38.25</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <v>191.25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>150</v>
+      </c>
+      <c r="G10" s="4" t="n">
+        <v>32.89</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <v>4933.5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="G9" s="4" t="n">
+      <c r="G11" s="4" t="n">
         <v>9.87</v>
       </c>
-      <c r="H9" s="4" t="n">
+      <c r="H11" s="4" t="n">
         <v>108.57</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="5" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="H12" s="5" t="n">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>44799</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <v>0.32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>